<commit_message>
Changes on 18th May
</commit_message>
<xml_diff>
--- a/Practice Data/Employee Sample Data.xlsx
+++ b/Practice Data/Employee Sample Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shiva\OneDrive\Desktop\Shiva\UiPath Coaching\Batch 4\UiPathTraining_Batch4\Practice Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34F2B45-8DD6-4169-970C-4ED03CA81918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42527B0C-C21F-4723-AA6A-D896667848BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{65C14963-D7D9-489F-85DF-B390E3AF6B64}"/>
   </bookViews>
@@ -1649,9 +1649,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1661,10 +1661,10 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16541,8 +16541,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>